<commit_message>
fixed example files. Still need to fix links
</commit_message>
<xml_diff>
--- a/inst/extdata/labelled.xlsx
+++ b/inst/extdata/labelled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/robert67_qut_edu_au/Documents/Documents/pcqolutilities/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{806E9974-6ECC-4FC2-B0EF-9D6F6EDCCA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{806E9974-6ECC-4FC2-B0EF-9D6F6EDCCA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFBE49D5-CCC2-4E97-861C-1021309018E0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{208A34A5-42C2-4F5F-9484-9F804A2F9CD5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{208A34A5-42C2-4F5F-9484-9F804A2F9CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="labelled" sheetId="1" r:id="rId1"/>
@@ -80,25 +80,25 @@
     <t>None of the time</t>
   </si>
   <si>
-    <t>Very, very worried</t>
-  </si>
-  <si>
-    <t>Very worried</t>
-  </si>
-  <si>
-    <t>Fairly worried</t>
-  </si>
-  <si>
-    <t>Somewhat worried</t>
-  </si>
-  <si>
-    <t>A little worried</t>
-  </si>
-  <si>
-    <t>Hardly worried</t>
-  </si>
-  <si>
-    <t>Not worried</t>
+    <t>Very, very worried/ concerned</t>
+  </si>
+  <si>
+    <t>Very worried/ concerned</t>
+  </si>
+  <si>
+    <t>Fairly worried/ concerned</t>
+  </si>
+  <si>
+    <t>Somewhat worried/ concerned</t>
+  </si>
+  <si>
+    <t>A little worried/ concerned</t>
+  </si>
+  <si>
+    <t>Hardly worried/ concerned</t>
+  </si>
+  <si>
+    <t>Not worried/ concerned</t>
   </si>
 </sst>
 </file>
@@ -473,10 +473,13 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>